<commit_message>
February - 1 commit
</commit_message>
<xml_diff>
--- a/7rmart/src/main/resources/TestData.xlsx
+++ b/7rmart/src/main/resources/TestData.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haikr\git\selenium\7rmart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3629D14-A161-4776-888D-7141D21715F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A98A8C-DA6E-466A-B818-4FE824B2D8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="MenuPage" sheetId="2" r:id="rId2"/>
-    <sheet name="AdminUsersPage" sheetId="3" r:id="rId3"/>
-    <sheet name="ManageDeliveryBoyPage" sheetId="4" r:id="rId4"/>
-    <sheet name="ManageLocationPage" sheetId="6" r:id="rId5"/>
-    <sheet name="ManageOfferCodePage" sheetId="5" r:id="rId6"/>
-    <sheet name="MobileSliderPage" sheetId="7" r:id="rId7"/>
+    <sheet name="ManageOrdersPage" sheetId="8" r:id="rId2"/>
+    <sheet name="MenuPage" sheetId="2" r:id="rId3"/>
+    <sheet name="AdminUsersPage" sheetId="3" r:id="rId4"/>
+    <sheet name="ManageDeliveryBoyPage" sheetId="4" r:id="rId5"/>
+    <sheet name="ManageLocationPage" sheetId="6" r:id="rId6"/>
+    <sheet name="ManageOfferCodePage" sheetId="5" r:id="rId7"/>
+    <sheet name="MobileSliderPage" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>admin</t>
   </si>
@@ -209,6 +210,9 @@
     <t>×
 Alert!
 User Created Successfully</t>
+  </si>
+  <si>
+    <t>Order Id</t>
   </si>
 </sst>
 </file>
@@ -609,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACCE1F3-5A20-4E94-8BEC-E59E9455C68A}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -679,6 +683,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8A00CA-5234-439D-8C71-DA57F3FBA0AE}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF612F5-E4E3-4C74-8824-4E6596061877}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -776,7 +844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF361CF-A0D9-48CE-8353-28FC994C59F5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -827,7 +895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21DAFE5-1216-4CDA-A7F9-6B220A1EE2DE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -870,7 +938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C8ABBE-6966-4DBA-B2C8-27D324B84A6E}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -949,7 +1017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCA222-CE40-44C8-A940-9E740A6C7C11}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1000,7 +1068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712595B7-7726-424D-9A55-1448FFE10E54}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
February - 5 commit
</commit_message>
<xml_diff>
--- a/7rmart/src/main/resources/TestData.xlsx
+++ b/7rmart/src/main/resources/TestData.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haikr\git\selenium\7rmart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A98A8C-DA6E-466A-B818-4FE824B2D8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BC3DBB-5436-4AFA-8B36-CB18BBE4930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="ManageOrdersPage" sheetId="8" r:id="rId2"/>
     <sheet name="MenuPage" sheetId="2" r:id="rId3"/>
-    <sheet name="AdminUsersPage" sheetId="3" r:id="rId4"/>
-    <sheet name="ManageDeliveryBoyPage" sheetId="4" r:id="rId5"/>
-    <sheet name="ManageLocationPage" sheetId="6" r:id="rId6"/>
-    <sheet name="ManageOfferCodePage" sheetId="5" r:id="rId7"/>
-    <sheet name="MobileSliderPage" sheetId="7" r:id="rId8"/>
+    <sheet name="ManageExpensePage" sheetId="9" r:id="rId4"/>
+    <sheet name="AdminUsersPage" sheetId="3" r:id="rId5"/>
+    <sheet name="ManageDeliveryBoyPage" sheetId="4" r:id="rId6"/>
+    <sheet name="ManageLocationPage" sheetId="6" r:id="rId7"/>
+    <sheet name="ManageOfferCodePage" sheetId="5" r:id="rId8"/>
+    <sheet name="PushNotificationPage" sheetId="11" r:id="rId9"/>
+    <sheet name="MobileSliderPage" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
   <si>
     <t>admin</t>
   </si>
@@ -214,12 +216,61 @@
   <si>
     <t>Order Id</t>
   </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Purchase Id</t>
+  </si>
+  <si>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Admin2(Admin)</t>
+  </si>
+  <si>
+    <t>IceCreams</t>
+  </si>
+  <si>
+    <t>Debit Cash</t>
+  </si>
+  <si>
+    <t>This is an expense of ice cream</t>
+  </si>
+  <si>
+    <t>×
+Alert!
+Expense Record Created Successfully</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Good Morning</t>
+  </si>
+  <si>
+    <t>This is a message for users</t>
+  </si>
+  <si>
+    <t>×
+Alert!
+Message send successfully</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +288,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -261,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -276,6 +333,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,11 +743,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712595B7-7726-424D-9A55-1448FFE10E54}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="54" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8A00CA-5234-439D-8C71-DA57F3FBA0AE}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
@@ -845,11 +941,100 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850252E-F145-4C7C-964E-40A6BBA2039D}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF361CF-A0D9-48CE-8353-28FC994C59F5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +1080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21DAFE5-1216-4CDA-A7F9-6B220A1EE2DE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -938,12 +1123,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C8ABBE-6966-4DBA-B2C8-27D324B84A6E}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,12 +1202,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCA222-CE40-44C8-A940-9E740A6C7C11}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,34 +1253,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712595B7-7726-424D-9A55-1448FFE10E54}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DCEA58-CE1D-47C3-9981-52EBBB38EA0A}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1"/>
-    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="54" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>49</v>
+      <c r="B3" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
February - 7 commit
</commit_message>
<xml_diff>
--- a/7rmart/src/main/resources/TestData.xlsx
+++ b/7rmart/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haikr\git\selenium\7rmart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BC3DBB-5436-4AFA-8B36-CB18BBE4930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D3F97F-94EA-44BC-A823-0A36BDF72771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>admin</t>
   </si>
@@ -264,6 +264,61 @@
     <t>×
 Alert!
 Message send successfully</t>
+  </si>
+  <si>
+    <t>Page Heading</t>
+  </si>
+  <si>
+    <t>List Pages</t>
+  </si>
+  <si>
+    <t>List Users</t>
+  </si>
+  <si>
+    <t>List Orders</t>
+  </si>
+  <si>
+    <t>List Expense</t>
+  </si>
+  <si>
+    <t>List Categories</t>
+  </si>
+  <si>
+    <t>List Products</t>
+  </si>
+  <si>
+    <t>List Offercodes</t>
+  </si>
+  <si>
+    <t>List Sliders</t>
+  </si>
+  <si>
+    <t>List Delivery Boy</t>
+  </si>
+  <si>
+    <t>List Locations</t>
+  </si>
+  <si>
+    <t>List Mobile Sliders</t>
+  </si>
+  <si>
+    <t>Time Field 1</t>
+  </si>
+  <si>
+    <t>Time Field 2</t>
+  </si>
+  <si>
+    <t>10:00am</t>
+  </si>
+  <si>
+    <t>6:30pm</t>
+  </si>
+  <si>
+    <t>Expected Text</t>
+  </si>
+  <si>
+    <t>01-Jan-1970
+05:00pm to 10:00pm</t>
   </si>
 </sst>
 </file>
@@ -780,58 +835,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8A00CA-5234-439D-8C71-DA57F3FBA0AE}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>148</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>141</v>
       </c>
@@ -844,99 +920,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF612F5-E4E3-4C74-8824-4E6596061877}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1085,7 +1207,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DCEA58-CE1D-47C3-9981-52EBBB38EA0A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
February 11 - commit
</commit_message>
<xml_diff>
--- a/7rmart/src/main/resources/TestData.xlsx
+++ b/7rmart/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haikr\git\selenium\7rmart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D3F97F-94EA-44BC-A823-0A36BDF72771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F08214-A8B7-45A4-BC2D-A7CA4F78C6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{9E743C28-A57C-4106-9A3F-A6821A63EAC5}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
   <si>
     <t>admin</t>
   </si>
@@ -300,25 +300,6 @@
   </si>
   <si>
     <t>List Mobile Sliders</t>
-  </si>
-  <si>
-    <t>Time Field 1</t>
-  </si>
-  <si>
-    <t>Time Field 2</t>
-  </si>
-  <si>
-    <t>10:00am</t>
-  </si>
-  <si>
-    <t>6:30pm</t>
-  </si>
-  <si>
-    <t>Expected Text</t>
-  </si>
-  <si>
-    <t>01-Jan-1970
-05:00pm to 10:00pm</t>
   </si>
 </sst>
 </file>
@@ -838,7 +819,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,29 +834,17 @@
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>148</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">

</xml_diff>